<commit_message>
Lista 5 na zajęcia
</commit_message>
<xml_diff>
--- a/Wyniki/Wyniki.xlsx
+++ b/Wyniki/Wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRz\Documents\Politechnika Rzeszowska Studenci\2018 lato\BazyDanychI4\Wyniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0901997F-08D1-40DA-A6F2-024A5D5CF176}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9FF42A06-34AB-462E-B2A7-CC0570645C6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,10 +156,10 @@
     <tableColumn id="6" xr3:uid="{61AA02F2-3FCD-4EFC-8D15-E648F15660B1}" name="Lab 2"/>
     <tableColumn id="7" xr3:uid="{FE6791A3-CBDC-45D5-AE17-43060192EB64}" name="Lista 3"/>
     <tableColumn id="8" xr3:uid="{7586B4CC-4010-47ED-9B83-F392376FFF3B}" name="Kartkówka 3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="%" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="%" dataDxfId="1">
       <calculatedColumnFormula>SUM(Tabela13[[#This Row],[Lista 1]:[Kartkówka 3]])/$B$33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Propozycja" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Propozycja" dataDxfId="0">
       <calculatedColumnFormula>IF(Tabela13[[#This Row],[%]]&lt;0.6, 2, IF(Tabela13[[#This Row],[%]]&lt;0.7, 3, IF(Tabela13[[#This Row],[%]]&lt;0.8, 3.5, IF(Tabela13[[#This Row],[%]]&lt;0.9, 4, IF(Tabela13[[#This Row],[%]]&lt;0.95, 4.5, 5)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,14 +838,14 @@
         <v>2</v>
       </c>
       <c r="H23">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="I23">
         <v>4.5</v>
       </c>
       <c r="J23">
         <f>SUM(Tabela13[[#This Row],[Lista 1]:[Kartkówka 3]])/$B$33</f>
-        <v>0.36666666666666664</v>
+        <v>0.39166666666666666</v>
       </c>
       <c r="K23">
         <f>IF(Tabela13[[#This Row],[%]]&lt;0.6, 2, IF(Tabela13[[#This Row],[%]]&lt;0.7, 3, IF(Tabela13[[#This Row],[%]]&lt;0.8, 3.5, IF(Tabela13[[#This Row],[%]]&lt;0.9, 4, IF(Tabela13[[#This Row],[%]]&lt;0.95, 4.5, 5)))))</f>

</xml_diff>